<commit_message>
Completed Official STO code. Need to convert to .exe
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -53,9 +53,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,94 +426,274 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.85546875" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="19.85546875" customWidth="1" min="3" max="4"/>
-    <col width="15.5703125" customWidth="1" min="5" max="5"/>
-    <col width="14.28515625" customWidth="1" min="6" max="6"/>
-    <col width="14.140625" customWidth="1" min="9" max="9"/>
+    <col width="5.42578125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.28515625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="11.5703125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="20.5703125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="16.42578125" customWidth="1" style="1" min="6" max="6"/>
+    <col width="14.85546875" customWidth="1" style="1" min="7" max="7"/>
+    <col width="9.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="9.85546875" customWidth="1" style="1" min="9" max="9"/>
+    <col width="14" customWidth="1" style="1" min="10" max="11"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" customFormat="1" s="2">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Auction Price</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Province</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Book (USD)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Canadian Price (CAD)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>US Price (USD)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Total US (USD)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>BOB</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>Exchange Rate</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>30000</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>BC</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" s="1" t="n">
         <v>25000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>32550</v>
       </c>
-      <c r="E2" t="n">
-        <v>23667</v>
-      </c>
       <c r="F2" t="n">
-        <v>26226.67</v>
+        <v>23667.1</v>
       </c>
       <c r="G2" t="n">
-        <v>1226.67</v>
-      </c>
-      <c r="I2" t="n">
+        <v>26226.77</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1226.77</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>0.7271</v>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>35000</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>BC</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>37800</v>
+      </c>
+      <c r="F3" t="n">
+        <v>27484.38</v>
+      </c>
+      <c r="G3" t="n">
+        <v>30082.22</v>
+      </c>
+      <c r="H3" t="n">
+        <v>82.22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>32500</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Alberta</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>31000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35175</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25575.74</v>
+      </c>
+      <c r="G4" t="n">
+        <v>28154.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-2845.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>38000</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Alberta</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40950</v>
+      </c>
+      <c r="F5" t="n">
+        <v>29774.74</v>
+      </c>
+      <c r="G5" t="n">
+        <v>32395.49</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2395.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>40000</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>Ontario</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>35000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>46330</v>
+      </c>
+      <c r="F6" t="n">
+        <v>33687</v>
+      </c>
+      <c r="G6" t="n">
+        <v>37457.87</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2457.87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>29500</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>Ontario</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>34465</v>
+      </c>
+      <c r="F7" t="n">
+        <v>25060</v>
+      </c>
+      <c r="G7" t="n">
+        <v>28744.6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3744.6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Ontario</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35030</v>
+      </c>
+      <c r="F8" t="n">
+        <v>25470</v>
+      </c>
+      <c r="G8" t="n">
+        <v>29158.7</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4158.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Book calculation fixed. Minor tweaks before exe
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nate\Desktop\Coding\Python Projects\Excel Practice\ExcelTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C7B49-B596-4F1F-B8FA-BE30ABD29EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA71CEA-D6A5-4A23-82AA-471665D796A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,8 +418,8 @@
     <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
     <col min="10" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="23" width="9.140625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -468,6 +468,34 @@
       <c r="G3"/>
       <c r="H3"/>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Changes to account for max_row issue
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nate\Desktop\Coding\Python Projects\Excel Practice\ExcelTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA71CEA-D6A5-4A23-82AA-471665D796A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6174983D-412C-486F-9F54-AF2C0EB3553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,8 +418,8 @@
     <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
     <col min="10" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="23" width="9.140625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="28" width="9.140625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -461,41 +461,6 @@
         <v>0.72709999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added Book conversion to python script
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -1,78 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nate\Desktop\Coding\Python Projects\Excel Practice\ExcelTest\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6174983D-412C-486F-9F54-AF2C0EB3553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="STO LLC Auction Calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="STO LLC Auction Calculations" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Auction Price</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Book (USD)</t>
-  </si>
-  <si>
-    <t>Canadian Price (CAD)</t>
-  </si>
-  <si>
-    <t>US Price (USD)</t>
-  </si>
-  <si>
-    <t>Total US (USD)</t>
-  </si>
-  <si>
-    <t>BOB</t>
-  </si>
-  <si>
-    <t>Exchange Rate</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -91,27 +54,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -399,66 +421,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="28" width="9.140625" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col width="4.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.85546875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15.28515625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="12.85546875" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12.5703125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="21" customWidth="1" style="1" min="6" max="6"/>
+    <col width="15.7109375" customWidth="1" style="1" min="7" max="7"/>
+    <col width="15" customWidth="1" style="1" min="8" max="8"/>
+    <col width="9.85546875" customWidth="1" style="1" min="9" max="9"/>
+    <col width="14" customWidth="1" style="1" min="10" max="11"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="31"/>
+    <col width="9.140625" customWidth="1" style="1" min="32" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="1" s="2">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Auction Price</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Province</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Book (CAD)</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Book (USD)</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Canadian Price (CAD)</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>US Price (USD)</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Total US (USD)</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>BOB</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Exchange Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="K2" s="1">
-        <v>0.72709999999999997</v>
+      <c r="B2" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>alb</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>32000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>23267.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>32550</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23667.1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>26226.77</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2959.57</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>0.7271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to amounts to reflect new auction destinations
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-24765" yWindow="2145" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="STO LLC Auction Calculations" sheetId="1" state="visible" r:id="rId1"/>
@@ -426,10 +426,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -444,8 +444,8 @@
     <col width="15" customWidth="1" style="1" min="8" max="8"/>
     <col width="9.85546875" customWidth="1" style="1" min="9" max="9"/>
     <col width="14" customWidth="1" style="1" min="10" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="31"/>
-    <col width="9.140625" customWidth="1" style="1" min="32" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="32"/>
+    <col width="9.140625" customWidth="1" style="1" min="33" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="2">
@@ -525,13 +525,44 @@
         <v>23667.1</v>
       </c>
       <c r="H2" t="n">
-        <v>26226.77</v>
+        <v>25923.77</v>
       </c>
       <c r="I2" t="n">
-        <v>-2959.57</v>
+        <v>-2656.57</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>0.7271</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>ont</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>32000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>23267.2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>35030</v>
+      </c>
+      <c r="G3" t="n">
+        <v>25470</v>
+      </c>
+      <c r="H3" t="n">
+        <v>27138.7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-3871.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made exe file v2
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -426,10 +426,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -444,8 +444,8 @@
     <col width="15" customWidth="1" style="1" min="8" max="8"/>
     <col width="9.85546875" customWidth="1" style="1" min="9" max="9"/>
     <col width="14" customWidth="1" style="1" min="10" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="32"/>
-    <col width="9.140625" customWidth="1" style="1" min="33" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="12" max="33"/>
+    <col width="9.140625" customWidth="1" style="1" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="2">
@@ -556,13 +556,44 @@
         <v>35030</v>
       </c>
       <c r="G3" t="n">
-        <v>25470</v>
+        <v>25470.31</v>
       </c>
       <c r="H3" t="n">
-        <v>27138.7</v>
+        <v>27139.01</v>
       </c>
       <c r="I3" t="n">
-        <v>-3871.5</v>
+        <v>-3871.81</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>30000</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>alb</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>32000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>23267.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>32550</v>
+      </c>
+      <c r="G4" t="n">
+        <v>23667.1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>25923.77</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-2656.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments made to convert from US book to CAD book
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -1,44 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nate\Desktop\Coding\Python Projects\Excel Practice\ExcelTest\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEAE9B6-4B06-4573-BFBB-098820FA50E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-24765" yWindow="2145" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="STO LLC Auction Calculations" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="STO LLC Auction Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Auction Price</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Book (USD)</t>
+  </si>
+  <si>
+    <t>Book (CAD)</t>
+  </si>
+  <si>
+    <t>Canadian Price (CAD)</t>
+  </si>
+  <si>
+    <t>US Price (USD)</t>
+  </si>
+  <si>
+    <t>Total US (USD)</t>
+  </si>
+  <si>
+    <t>BOB</t>
+  </si>
+  <si>
+    <t>Exchange Rate</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -53,87 +99,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,179 +414,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="4.5703125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="13.85546875" customWidth="1" style="1" min="2" max="2"/>
-    <col width="15.28515625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="12.85546875" customWidth="1" style="1" min="4" max="4"/>
-    <col width="12.5703125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="21" customWidth="1" style="1" min="6" max="6"/>
-    <col width="15.7109375" customWidth="1" style="1" min="7" max="7"/>
-    <col width="15" customWidth="1" style="1" min="8" max="8"/>
-    <col width="9.85546875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="14" customWidth="1" style="1" min="10" max="11"/>
-    <col width="9.140625" customWidth="1" style="1" min="12" max="33"/>
-    <col width="9.140625" customWidth="1" style="1" min="34" max="16384"/>
+    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="14" style="1" customWidth="1"/>
+    <col min="12" max="37" width="9.140625" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="2">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Auction Price</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Province</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Book (CAD)</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Book (USD)</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Canadian Price (CAD)</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>US Price (USD)</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Total US (USD)</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>BOB</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Exchange Rate</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>30000</v>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>alb</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>32000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>23267.2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>32550</v>
-      </c>
-      <c r="G2" t="n">
-        <v>23667.1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>25923.77</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-2656.57</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>0.7271</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>ont</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>32000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>23267.2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>35030</v>
-      </c>
-      <c r="G3" t="n">
-        <v>25470.31</v>
-      </c>
-      <c r="H3" t="n">
-        <v>27139.01</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-3871.81</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>30000</v>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>alb</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>32000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>23267.2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>32550</v>
-      </c>
-      <c r="G4" t="n">
-        <v>23667.1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>25923.77</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-2656.57</v>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added both exchange rates. Changed specific calculations
</commit_message>
<xml_diff>
--- a/STO_BOB.xlsx
+++ b/STO_BOB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nate\Desktop\Coding\Python Projects\Excel Practice\ExcelTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEAE9B6-4B06-4573-BFBB-098820FA50E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F8AC31-E3B7-4837-8153-AA06A0E1CC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24075" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STO LLC Auction Calculations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -49,7 +49,10 @@
     <t>BOB</t>
   </si>
   <si>
-    <t>Exchange Rate</t>
+    <t>CAD =&gt; USD %</t>
+  </si>
+  <si>
+    <t>USD =&gt; CAD %</t>
   </si>
 </sst>
 </file>
@@ -73,18 +76,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,18 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -415,58 +406,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="37" width="9.140625" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="2" customWidth="1"/>
+    <col min="10" max="12" width="14" style="2" customWidth="1"/>
+    <col min="13" max="40" width="9.140625" style="2" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="K2" s="2">
+        <v>0.7218</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>